<commit_message>
starting to update the roster
</commit_message>
<xml_diff>
--- a/src/assets/tookachi/roster.xlsx
+++ b/src/assets/tookachi/roster.xlsx
@@ -1,37 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\workspace\ihadojo\src\assets\tookhachi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahendry/Code/ihadojo-rewrite/src/assets/tookachi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73BBF60-B2DA-4E0F-8EAD-251AC3B751D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62A2396-C9D4-A64C-8522-3880C87DE427}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2166" yWindow="2166" windowWidth="17280" windowHeight="8994" xr2:uid="{270A1642-C05E-43BC-94F4-89FE0A2FED94}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="9000" xr2:uid="{270A1642-C05E-43BC-94F4-89FE0A2FED94}"/>
   </bookViews>
   <sheets>
     <sheet name="roster" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">roster!$A$1:$H$48</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="114">
   <si>
     <t>dojo</t>
   </si>
@@ -243,7 +240,136 @@
     <t>seikichiiha.jpg</t>
   </si>
   <si>
-    <t>Hanshi, 10</t>
+    <t>Kass</t>
+  </si>
+  <si>
+    <t>Alaska Shido-kan</t>
+  </si>
+  <si>
+    <t>Kenai, Alaska</t>
+  </si>
+  <si>
+    <t>Sandy</t>
+  </si>
+  <si>
+    <t>sandykass.jpg</t>
+  </si>
+  <si>
+    <t>Keeven</t>
+  </si>
+  <si>
+    <t>Macik</t>
+  </si>
+  <si>
+    <t>Hannele</t>
+  </si>
+  <si>
+    <t>Zubeck</t>
+  </si>
+  <si>
+    <t>hannelezubeck.jpg</t>
+  </si>
+  <si>
+    <t>Maija</t>
+  </si>
+  <si>
+    <t>jimkass.JPG</t>
+  </si>
+  <si>
+    <t>keevenmacik.JPG</t>
+  </si>
+  <si>
+    <t>maijazubeck.JPG</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <t>Curtis</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Pangelinan</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Flax</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Coursey</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Margot</t>
+  </si>
+  <si>
+    <t>Paz</t>
+  </si>
+  <si>
+    <t>Mom</t>
+  </si>
+  <si>
+    <t>Noell</t>
+  </si>
+  <si>
+    <t>Dunlap McMichael</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>McMichael</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Reese</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>Hudson</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>McCloskey</t>
+  </si>
+  <si>
+    <t>Alexandria, Virginia</t>
+  </si>
+  <si>
+    <t>Lorton, Virginia</t>
+  </si>
+  <si>
+    <t>Arlington, Virginia</t>
+  </si>
+  <si>
+    <t>Burke, Virginia</t>
+  </si>
+  <si>
+    <t>Gaithersburg, Maryland</t>
   </si>
 </sst>
 </file>
@@ -595,21 +721,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A3967E-334D-4DA9-9EB0-62515739C97A}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.26171875" customWidth="1"/>
-    <col min="3" max="3" width="16.47265625" customWidth="1"/>
-    <col min="4" max="4" width="24.47265625" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -635,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -651,8 +778,8 @@
       <c r="E2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
-        <v>70</v>
+      <c r="F2">
+        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -661,7 +788,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -684,7 +811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -701,7 +828,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -724,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -747,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -770,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -793,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -816,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -839,7 +966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -862,7 +989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -885,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -908,7 +1035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -931,7 +1058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -954,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -977,7 +1104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1000,7 +1127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1023,7 +1150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1046,7 +1173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1069,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1092,7 +1219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1115,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1138,7 +1265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1161,7 +1288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1207,7 +1334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1256,7 +1383,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1273,7 +1400,442 @@
         <v>62</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H48" xr:uid="{8D7DD68C-45B6-194C-97D4-AA8A4AA96481}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add canada roster photos
</commit_message>
<xml_diff>
--- a/src/assets/tookachi/roster.xlsx
+++ b/src/assets/tookachi/roster.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahendry/Code/ihadojo-rewrite/src/assets/tookachi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahendry\workspace\ihadojo.com\src\assets\tookachi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474DFAFC-EDB2-F446-8376-84F4A7E1D49A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="1500" windowWidth="17280" windowHeight="9000" xr2:uid="{270A1642-C05E-43BC-94F4-89FE0A2FED94}"/>
+    <workbookView xWindow="6960" yWindow="1500" windowWidth="17280" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="roster" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">roster!$A$1:$H$48</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="155">
   <si>
     <t>dojo</t>
   </si>
@@ -412,12 +411,93 @@
   </si>
   <si>
     <t>robertpangelinan.png</t>
+  </si>
+  <si>
+    <t>Fortunato</t>
+  </si>
+  <si>
+    <t>Restagno</t>
+  </si>
+  <si>
+    <t>Grand River Karate</t>
+  </si>
+  <si>
+    <t>Waterloo, Ontario</t>
+  </si>
+  <si>
+    <t>Fortunato_Restagno.jpg</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Cowen</t>
+  </si>
+  <si>
+    <t>Doug_Cowan.jpg</t>
+  </si>
+  <si>
+    <t>Klaus</t>
+  </si>
+  <si>
+    <t>Stegner</t>
+  </si>
+  <si>
+    <t>Klaus_Stegner.jpg</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Bob_Davis.jpg</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Jessup</t>
+  </si>
+  <si>
+    <t>Steven_Jessup.jpg</t>
+  </si>
+  <si>
+    <t>Tricia</t>
+  </si>
+  <si>
+    <t>Burbidge</t>
+  </si>
+  <si>
+    <t>Tricia_Burbidge.jpg</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>McKechnie</t>
+  </si>
+  <si>
+    <t>Megan_McKechnie.jpg</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Dave_Marks.jpg</t>
+  </si>
+  <si>
+    <t>Laura_Marks.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,7 +515,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -443,12 +523,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,23 +866,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A3967E-334D-4DA9-9EB0-62515739C97A}">
-  <dimension ref="A1:H48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -804,7 +909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -830,7 +935,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -853,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -870,7 +975,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -893,7 +998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -916,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -939,7 +1044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -962,7 +1067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -985,7 +1090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1008,7 +1113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1031,7 +1136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1054,7 +1159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1100,7 +1205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1123,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1146,7 +1251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1169,7 +1274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1192,7 +1297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1215,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1238,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1261,7 +1366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1284,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1307,7 +1412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1330,7 +1435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1353,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1376,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1399,7 +1504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1425,7 +1530,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1442,7 +1547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1468,7 +1573,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -1488,7 +1593,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1514,7 +1619,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1540,7 +1645,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -1566,7 +1671,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -1592,7 +1697,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -1618,7 +1723,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -1644,7 +1749,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -1670,7 +1775,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -1696,7 +1801,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -1722,7 +1827,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -1748,7 +1853,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -1768,7 +1873,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -1794,7 +1899,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -1814,7 +1919,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -1840,7 +1945,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>102</v>
       </c>
@@ -1866,7 +1971,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -1892,7 +1997,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -1918,8 +2023,239 @@
         <v>123</v>
       </c>
     </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="2">
+        <v>6</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50" s="2">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F51" s="2">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F52" s="2">
+        <v>3</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F53" s="2">
+        <v>2</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F56" s="2">
+        <v>4</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H48" xr:uid="{8D7DD68C-45B6-194C-97D4-AA8A4AA96481}"/>
+  <autoFilter ref="A1:H48"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove package registration, update roster
</commit_message>
<xml_diff>
--- a/src/assets/tookachi/roster.xlsx
+++ b/src/assets/tookachi/roster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="512">
   <si>
     <t>dojo</t>
   </si>
@@ -1605,6 +1605,12 @@
   </si>
   <si>
     <t>Lauren Moran.jpg</t>
+  </si>
+  <si>
+    <t>Kaitlin</t>
+  </si>
+  <si>
+    <t>Kaitlin Moran.jpg</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="H154" sqref="H154"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="K156" sqref="K156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6005,7 +6011,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>474</v>
+        <v>510</v>
       </c>
       <c r="B154" t="s">
         <v>475</v>
@@ -6020,15 +6026,15 @@
         <v>60</v>
       </c>
       <c r="H154" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B155" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C155" t="s">
         <v>470</v>
@@ -6039,22 +6045,16 @@
       <c r="E155" t="s">
         <v>60</v>
       </c>
-      <c r="F155">
-        <v>8</v>
-      </c>
-      <c r="G155" t="s">
-        <v>3</v>
-      </c>
       <c r="H155" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B156" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C156" t="s">
         <v>470</v>
@@ -6065,16 +6065,22 @@
       <c r="E156" t="s">
         <v>60</v>
       </c>
+      <c r="F156">
+        <v>8</v>
+      </c>
+      <c r="G156" t="s">
+        <v>3</v>
+      </c>
       <c r="H156" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B157" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="C157" t="s">
         <v>470</v>
@@ -6086,12 +6092,12 @@
         <v>60</v>
       </c>
       <c r="H157" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>165</v>
+        <v>479</v>
       </c>
       <c r="B158" t="s">
         <v>472</v>
@@ -6105,19 +6111,13 @@
       <c r="E158" t="s">
         <v>60</v>
       </c>
-      <c r="F158">
-        <v>8</v>
-      </c>
-      <c r="G158" t="s">
-        <v>3</v>
-      </c>
       <c r="H158" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="B159" t="s">
         <v>472</v>
@@ -6132,18 +6132,18 @@
         <v>60</v>
       </c>
       <c r="F159">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G159" t="s">
         <v>3</v>
       </c>
       <c r="H159" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>480</v>
+        <v>204</v>
       </c>
       <c r="B160" t="s">
         <v>472</v>
@@ -6157,16 +6157,22 @@
       <c r="E160" t="s">
         <v>60</v>
       </c>
+      <c r="F160">
+        <v>5</v>
+      </c>
+      <c r="G160" t="s">
+        <v>3</v>
+      </c>
       <c r="H160" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B161" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="C161" t="s">
         <v>470</v>
@@ -6177,19 +6183,13 @@
       <c r="E161" t="s">
         <v>60</v>
       </c>
-      <c r="F161">
-        <v>3</v>
-      </c>
-      <c r="G161" t="s">
-        <v>4</v>
-      </c>
       <c r="H161" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B162" t="s">
         <v>482</v>
@@ -6204,21 +6204,21 @@
         <v>60</v>
       </c>
       <c r="F162">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G162" t="s">
         <v>4</v>
       </c>
       <c r="H162" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B163" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C163" t="s">
         <v>470</v>
@@ -6236,12 +6236,12 @@
         <v>4</v>
       </c>
       <c r="H163" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B164" t="s">
         <v>485</v>
@@ -6259,18 +6259,18 @@
         <v>2</v>
       </c>
       <c r="G164" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H164" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B165" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C165" t="s">
         <v>470</v>
@@ -6282,21 +6282,21 @@
         <v>60</v>
       </c>
       <c r="F165">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G165" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H165" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B166" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C166" t="s">
         <v>470</v>
@@ -6307,13 +6307,19 @@
       <c r="E166" t="s">
         <v>60</v>
       </c>
+      <c r="F166">
+        <v>7</v>
+      </c>
+      <c r="G166" t="s">
+        <v>4</v>
+      </c>
       <c r="H166" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B167" t="s">
         <v>490</v>
@@ -6328,15 +6334,15 @@
         <v>60</v>
       </c>
       <c r="H167" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B168" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C168" t="s">
         <v>470</v>
@@ -6347,13 +6353,33 @@
       <c r="E168" t="s">
         <v>60</v>
       </c>
-      <c r="F168">
+      <c r="H168" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>492</v>
+      </c>
+      <c r="B169" t="s">
+        <v>493</v>
+      </c>
+      <c r="C169" t="s">
+        <v>470</v>
+      </c>
+      <c r="D169" t="s">
+        <v>473</v>
+      </c>
+      <c r="E169" t="s">
+        <v>60</v>
+      </c>
+      <c r="F169">
         <v>7</v>
       </c>
-      <c r="G168" t="s">
-        <v>3</v>
-      </c>
-      <c r="H168" t="s">
+      <c r="G169" t="s">
+        <v>3</v>
+      </c>
+      <c r="H169" t="s">
         <v>505</v>
       </c>
     </row>

</xml_diff>